<commit_message>
BUG: Fix read_excel w/parse_cols & empty dataset
Closes gh-9208.
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/test1.xlsx
+++ b/pandas/tests/io/data/test1.xlsx
@@ -1,14 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beano\Repositories\pandas\pandas\tests\io\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A80AB08-DD4C-4F74-A488-F01DCF0B07AA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="-20" windowWidth="29560" windowHeight="24100" tabRatio="500"/>
+    <workbookView xWindow="84" yWindow="-24" windowWidth="29556" windowHeight="24096" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
@@ -48,12 +55,18 @@
   <si>
     <t>ignore</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -93,6 +106,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,17 +438,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>35066</v>
       </c>
@@ -458,7 +479,7 @@
         <v>-1.1597380616899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>35067</v>
       </c>
@@ -475,7 +496,7 @@
         <v>0.212549316967</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>35068</v>
       </c>
@@ -492,7 +513,7 @@
         <v>1.3462704195199999</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>35069</v>
       </c>
@@ -509,7 +530,7 @@
         <v>0.67525259227000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>35070</v>
       </c>
@@ -526,7 +547,7 @@
         <v>0.103468562917</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>35073</v>
       </c>
@@ -543,7 +564,7 @@
         <v>1.0627820613000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>35074</v>
       </c>
@@ -563,7 +584,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -573,16 +594,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
       <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -610,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>35066</v>
       </c>
@@ -627,7 +648,7 @@
         <v>-1.1597380616899999</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>35067</v>
       </c>
@@ -644,7 +665,7 @@
         <v>0.212549316967</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>35068</v>
       </c>
@@ -661,7 +682,7 @@
         <v>1.3462704195199999</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>35069</v>
       </c>
@@ -678,7 +699,7 @@
         <v>0.67525259227000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>35070</v>
       </c>
@@ -695,7 +716,7 @@
         <v>0.103468562917</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>35073</v>
       </c>
@@ -712,7 +733,7 @@
         <v>1.0627820613000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>35074</v>
       </c>
@@ -732,11 +753,46 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4669757C-F7B6-4CFC-9F46-A8DF37DF746B}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TST: Test unnamed columns with index_col for Excel
Closes gh-18792.
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/test1.xlsx
+++ b/pandas/tests/io/data/test1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beano\Repositories\pandas\pandas\tests\io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A80AB08-DD4C-4F74-A488-F01DCF0B07AA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9007CB-C74A-4E7F-8E16-6EDF2B37F435}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84" yWindow="-24" windowWidth="29556" windowHeight="24096" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="84" yWindow="-24" windowWidth="29556" windowHeight="24096" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>A</t>
   </si>
@@ -61,13 +62,37 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>col1</t>
+  </si>
+  <si>
+    <t>col2</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -75,6 +100,14 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -93,13 +126,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4669757C-F7B6-4CFC-9F46-A8DF37DF746B}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -795,4 +846,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624CF529-5128-482A-A33B-732E2FE6972F}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>